<commit_message>
Changes to be committed: 	modified:   nepse_data.xlsx 	deleted:    step0.png 	deleted:    step1.png 	deleted:    step2.png 	deleted:    step3.png 	deleted:    step4.png 	modified:   test.js
</commit_message>
<xml_diff>
--- a/nepse_data.xlsx
+++ b/nepse_data.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F94"/>
+  <dimension ref="A1:F93"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -424,1852 +424,1847 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>No data available</v>
+        <v>B1</v>
+      </c>
+      <c r="B2" t="str">
+        <v>RADHI/39729/807.44</v>
+      </c>
+      <c r="C2" t="str">
+        <v>CHDC/11955/2,607.03</v>
+      </c>
+      <c r="D2" t="str">
+        <v>NRN/15213/2,030.98</v>
+      </c>
+      <c r="E2" t="str">
+        <v>NIFRA/93958/283.12</v>
+      </c>
+      <c r="F2" t="str">
+        <v>SHIVM/47132/521.86</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>B1</v>
+        <v>B3</v>
       </c>
       <c r="B3" t="str">
-        <v>RADHI/39729/807.44</v>
+        <v>SHIVM/18991/528.19</v>
       </c>
       <c r="C3" t="str">
-        <v>CHDC/11955/2,607.03</v>
+        <v>OMPL/6520/1,575.65</v>
       </c>
       <c r="D3" t="str">
-        <v>NRN/15213/2,030.98</v>
+        <v>MBL/38448/220.89</v>
       </c>
       <c r="E3" t="str">
-        <v>NIFRA/93958/283.12</v>
+        <v>HLI/19300/405.47</v>
       </c>
       <c r="F3" t="str">
-        <v>SHIVM/47132/521.86</v>
+        <v>PRVU/24310/208.18</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>B3</v>
+        <v>B4</v>
       </c>
       <c r="B4" t="str">
-        <v>SHIVM/18991/528.19</v>
+        <v>SARBTM/71072/844.96</v>
       </c>
       <c r="C4" t="str">
-        <v>OMPL/6520/1,575.65</v>
+        <v>HRL/40608/934.13</v>
       </c>
       <c r="D4" t="str">
-        <v>MBL/38448/220.89</v>
+        <v>UMRH/44446/610.21</v>
       </c>
       <c r="E4" t="str">
-        <v>HLI/19300/405.47</v>
+        <v>GMFIL/43531/492.25</v>
       </c>
       <c r="F4" t="str">
-        <v>PRVU/24310/208.18</v>
+        <v>API/57495/300.99</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>B4</v>
+        <v>B5</v>
       </c>
       <c r="B5" t="str">
-        <v>SARBTM/71072/844.96</v>
+        <v>HIDCLP/109453/211.79</v>
       </c>
       <c r="C5" t="str">
-        <v>HRL/40608/934.13</v>
+        <v>HRL/12099/955.22</v>
       </c>
       <c r="D5" t="str">
-        <v>UMRH/44446/610.21</v>
+        <v>CHDC/4557/2,611.51</v>
       </c>
       <c r="E5" t="str">
-        <v>GMFIL/43531/492.25</v>
+        <v>NGPL/27815/392.55</v>
       </c>
       <c r="F5" t="str">
-        <v>API/57495/300.99</v>
+        <v>LBBL/17067/446.39</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>B5</v>
+        <v>B6</v>
       </c>
       <c r="B6" t="str">
-        <v>HIDCLP/109453/211.79</v>
+        <v>NRIC/511570/1,296.22</v>
       </c>
       <c r="C6" t="str">
-        <v>HRL/12099/955.22</v>
+        <v>UPCL/167968/447.39</v>
       </c>
       <c r="D6" t="str">
-        <v>CHDC/4557/2,611.51</v>
+        <v>RIDI/168796/278.28</v>
       </c>
       <c r="E6" t="str">
-        <v>NGPL/27815/392.55</v>
+        <v>HRL/49334/946.85</v>
       </c>
       <c r="F6" t="str">
-        <v>LBBL/17067/446.39</v>
+        <v>HIDCLP/151839/210.92</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>B6</v>
+        <v>B7</v>
       </c>
       <c r="B7" t="str">
-        <v>NRIC/511570/1,296.22</v>
+        <v>NRN/16333/2,047.66</v>
       </c>
       <c r="C7" t="str">
-        <v>UPCL/167968/447.39</v>
+        <v>CHDC/10817/2,591.12</v>
       </c>
       <c r="D7" t="str">
-        <v>RIDI/168796/278.28</v>
+        <v>RADHI/23887/788.81</v>
       </c>
       <c r="E7" t="str">
-        <v>HRL/49334/946.85</v>
+        <v>GHL/44340/257.69</v>
       </c>
       <c r="F7" t="str">
-        <v>HIDCLP/151839/210.92</v>
+        <v>SIFC/17770/576.10</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="str">
-        <v>B7</v>
+        <v>B8</v>
       </c>
       <c r="B8" t="str">
-        <v>NRN/16333/2,047.66</v>
+        <v>NGPL/219265/406.27</v>
       </c>
       <c r="C8" t="str">
-        <v>CHDC/10817/2,591.12</v>
+        <v>HIDCLP/169023/214.09</v>
       </c>
       <c r="D8" t="str">
-        <v>RADHI/23887/788.81</v>
+        <v>SADBL/66870/427.03</v>
       </c>
       <c r="E8" t="str">
-        <v>GHL/44340/257.69</v>
+        <v>SAHAS/49699/557.32</v>
       </c>
       <c r="F8" t="str">
-        <v>SIFC/17770/576.10</v>
+        <v>LSL/107199/223.82</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="str">
-        <v>B8</v>
+        <v>B10</v>
       </c>
       <c r="B9" t="str">
-        <v>NGPL/219265/406.27</v>
+        <v>HIDCLP/79410/213.63</v>
       </c>
       <c r="C9" t="str">
-        <v>HIDCLP/169023/214.09</v>
+        <v>SHPC/16460/626.69</v>
       </c>
       <c r="D9" t="str">
-        <v>SADBL/66870/427.03</v>
+        <v>CIT/3559/1,921.25</v>
       </c>
       <c r="E9" t="str">
-        <v>SAHAS/49699/557.32</v>
+        <v>NTC/7525/871.57</v>
       </c>
       <c r="F9" t="str">
-        <v>LSL/107199/223.82</v>
+        <v>CHCL/9438/576.65</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="str">
-        <v>B10</v>
+        <v>B11</v>
       </c>
       <c r="B10" t="str">
-        <v>HIDCLP/79410/213.63</v>
+        <v>NABIL/16858/497.17</v>
       </c>
       <c r="C10" t="str">
-        <v>SHPC/16460/626.69</v>
+        <v>RHPL/15356/413.79</v>
       </c>
       <c r="D10" t="str">
-        <v>CIT/3559/1,921.25</v>
+        <v>CIT/3220/1,910.72</v>
       </c>
       <c r="E10" t="str">
-        <v>NTC/7525/871.57</v>
+        <v>ALICL/7896/659.16</v>
       </c>
       <c r="F10" t="str">
-        <v>CHCL/9438/576.65</v>
+        <v>SINDU/6382/844.66</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="str">
-        <v>B11</v>
+        <v>B13</v>
       </c>
       <c r="B11" t="str">
-        <v>NABIL/16858/497.17</v>
+        <v>BPCL/24724/702.00</v>
       </c>
       <c r="C11" t="str">
-        <v>RHPL/15356/413.79</v>
+        <v>UMHL/26140/520.29</v>
       </c>
       <c r="D11" t="str">
-        <v>CIT/3220/1,910.72</v>
+        <v>CORBL/3913/2,542.93</v>
       </c>
       <c r="E11" t="str">
-        <v>ALICL/7896/659.16</v>
+        <v>NGPL/26382/392.01</v>
       </c>
       <c r="F11" t="str">
-        <v>SINDU/6382/844.66</v>
+        <v>HRL/8464/973.13</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="str">
-        <v>B13</v>
+        <v>B14</v>
       </c>
       <c r="B12" t="str">
-        <v>BPCL/24724/702.00</v>
+        <v>CGH/51941/927.87</v>
       </c>
       <c r="C12" t="str">
-        <v>UMHL/26140/520.29</v>
+        <v>HRL/36173/941.31</v>
       </c>
       <c r="D12" t="str">
-        <v>CORBL/3913/2,542.93</v>
+        <v>HIDCLP/137778/211.41</v>
       </c>
       <c r="E12" t="str">
-        <v>NGPL/26382/392.01</v>
+        <v>CHCL/43140/577.14</v>
       </c>
       <c r="F12" t="str">
-        <v>HRL/8464/973.13</v>
+        <v>SAHAS/44876/537.46</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="str">
-        <v>B14</v>
+        <v>B16</v>
       </c>
       <c r="B13" t="str">
-        <v>CGH/51941/927.87</v>
+        <v>RADHI/119060/817.97</v>
       </c>
       <c r="C13" t="str">
-        <v>HRL/36173/941.31</v>
+        <v>CHDC/30520/2,697.51</v>
       </c>
       <c r="D13" t="str">
-        <v>HIDCLP/137778/211.41</v>
+        <v>CREST/16644/1,815.47</v>
       </c>
       <c r="E13" t="str">
-        <v>CHCL/43140/577.14</v>
+        <v>NMIC/15864/1,842.98</v>
       </c>
       <c r="F13" t="str">
-        <v>SAHAS/44876/537.46</v>
+        <v>SHL/52860/567.26</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="str">
-        <v>B16</v>
+        <v>B17</v>
       </c>
       <c r="B14" t="str">
-        <v>RADHI/119060/817.97</v>
+        <v>NGPL/419689/400.85</v>
       </c>
       <c r="C14" t="str">
-        <v>CHDC/30520/2,697.51</v>
+        <v>HIDCLP/575031/216.05</v>
       </c>
       <c r="D14" t="str">
-        <v>CREST/16644/1,815.47</v>
+        <v>HIDCL/211702/312.52</v>
       </c>
       <c r="E14" t="str">
-        <v>NMIC/15864/1,842.98</v>
+        <v>MEN/85008/616.51</v>
       </c>
       <c r="F14" t="str">
-        <v>SHL/52860/567.26</v>
+        <v>SPDL/77517/413.80</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="str">
-        <v>B17</v>
+        <v>B18</v>
       </c>
       <c r="B15" t="str">
-        <v>NGPL/419689/400.85</v>
+        <v>SPIL/23584/814.90</v>
       </c>
       <c r="C15" t="str">
-        <v>HIDCLP/575031/216.05</v>
+        <v>RADHI/16065/801.46</v>
       </c>
       <c r="D15" t="str">
-        <v>HIDCL/211702/312.52</v>
+        <v>NLICL/19339/611.26</v>
       </c>
       <c r="E15" t="str">
-        <v>MEN/85008/616.51</v>
+        <v>NLIC/12855/752.94</v>
       </c>
       <c r="F15" t="str">
-        <v>SPDL/77517/413.80</v>
+        <v>NRN/4527/2,040.05</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="str">
-        <v>B18</v>
+        <v>B19</v>
       </c>
       <c r="B16" t="str">
-        <v>SPIL/23584/814.90</v>
+        <v>BPCL/111187/646.16</v>
       </c>
       <c r="C16" t="str">
-        <v>RADHI/16065/801.46</v>
+        <v>CHDC/9482/2,661.98</v>
       </c>
       <c r="D16" t="str">
-        <v>NLICL/19339/611.26</v>
+        <v>LBBL/31857/464.86</v>
       </c>
       <c r="E16" t="str">
-        <v>NLIC/12855/752.94</v>
+        <v>NADEP/15386/850.57</v>
       </c>
       <c r="F16" t="str">
-        <v>NRN/4527/2,040.05</v>
+        <v>OMPL/6035/1,765.64</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="str">
-        <v>B19</v>
+        <v>B20</v>
       </c>
       <c r="B17" t="str">
-        <v>BPCL/111187/646.16</v>
+        <v>CHDC/7716/2,572.49</v>
       </c>
       <c r="C17" t="str">
-        <v>CHDC/9482/2,661.98</v>
+        <v>SHPC/28022/616.29</v>
       </c>
       <c r="D17" t="str">
-        <v>LBBL/31857/464.86</v>
+        <v>SHIVM/29759/523.07</v>
       </c>
       <c r="E17" t="str">
-        <v>NADEP/15386/850.57</v>
+        <v>RADHI/18805/798.24</v>
       </c>
       <c r="F17" t="str">
-        <v>OMPL/6035/1,765.64</v>
+        <v>EBL/20076/657.36</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="str">
-        <v>B20</v>
+        <v>B21</v>
       </c>
       <c r="B18" t="str">
-        <v>CHDC/7716/2,572.49</v>
+        <v>SHIVM/57353/521.59</v>
       </c>
       <c r="C18" t="str">
-        <v>SHPC/28022/616.29</v>
+        <v>SHPC/42026/608.15</v>
       </c>
       <c r="D18" t="str">
-        <v>SHIVM/29759/523.07</v>
+        <v>SMHL/18266/1,059.98</v>
       </c>
       <c r="E18" t="str">
-        <v>RADHI/18805/798.24</v>
+        <v>HIDCLP/79337/218.12</v>
       </c>
       <c r="F18" t="str">
-        <v>EBL/20076/657.36</v>
+        <v>HIDCL/39566/306.84</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="str">
-        <v>B21</v>
+        <v>B22</v>
       </c>
       <c r="B19" t="str">
-        <v>SHIVM/57353/521.59</v>
+        <v>UPCL/85415/455.50</v>
       </c>
       <c r="C19" t="str">
-        <v>SHPC/42026/608.15</v>
+        <v>SHIVM/55086/525.82</v>
       </c>
       <c r="D19" t="str">
-        <v>SMHL/18266/1,059.98</v>
+        <v>KPCL/40380/553.91</v>
       </c>
       <c r="E19" t="str">
-        <v>HIDCLP/79337/218.12</v>
+        <v>GHL/76179/259.87</v>
       </c>
       <c r="F19" t="str">
-        <v>HIDCL/39566/306.84</v>
+        <v>UNHPL/35020/389.48</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="str">
-        <v>B22</v>
+        <v>B25</v>
       </c>
       <c r="B20" t="str">
-        <v>UPCL/85415/455.50</v>
+        <v>KBL/195292/215.04</v>
       </c>
       <c r="C20" t="str">
-        <v>SHIVM/55086/525.82</v>
+        <v>SHPC/33009/620.51</v>
       </c>
       <c r="D20" t="str">
-        <v>KPCL/40380/553.91</v>
+        <v>HIDCL/65469/307.80</v>
       </c>
       <c r="E20" t="str">
-        <v>GHL/76179/259.87</v>
+        <v>NGPL/40583/399.79</v>
       </c>
       <c r="F20" t="str">
-        <v>UNHPL/35020/389.48</v>
+        <v>NRN/8996/2,048.96</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="str">
-        <v>B25</v>
+        <v>B26</v>
       </c>
       <c r="B21" t="str">
-        <v>KBL/195292/215.04</v>
+        <v>RADHI/125376/801.41</v>
       </c>
       <c r="C21" t="str">
-        <v>SHPC/33009/620.51</v>
+        <v>LBBL/55387/456.45</v>
       </c>
       <c r="D21" t="str">
-        <v>HIDCL/65469/307.80</v>
+        <v>NGPL/58586/391.77</v>
       </c>
       <c r="E21" t="str">
-        <v>NGPL/40583/399.79</v>
+        <v>SHIVM/31230/523.52</v>
       </c>
       <c r="F21" t="str">
-        <v>NRN/8996/2,048.96</v>
+        <v>NLIC/20531/757.19</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="str">
-        <v>B26</v>
+        <v>B28</v>
       </c>
       <c r="B22" t="str">
-        <v>RADHI/125376/801.41</v>
+        <v>SAHAS/104199/535.34</v>
       </c>
       <c r="C22" t="str">
-        <v>LBBL/55387/456.45</v>
+        <v>NIFRA/122748/286.06</v>
       </c>
       <c r="D22" t="str">
-        <v>NGPL/58586/391.77</v>
+        <v>MNBBL/81503/361.26</v>
       </c>
       <c r="E22" t="str">
-        <v>SHIVM/31230/523.52</v>
+        <v>CORBL/9666/2,422.47</v>
       </c>
       <c r="F22" t="str">
-        <v>NLIC/20531/757.19</v>
+        <v>UNHPL/53220/398.10</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="str">
-        <v>B28</v>
+        <v>B29</v>
       </c>
       <c r="B23" t="str">
-        <v>SAHAS/104199/535.34</v>
+        <v>BPCL/108792/690.85</v>
       </c>
       <c r="C23" t="str">
-        <v>NIFRA/122748/286.06</v>
+        <v>GRDBL/19732/1,267.53</v>
       </c>
       <c r="D23" t="str">
-        <v>MNBBL/81503/361.26</v>
+        <v>CHDC/7028/2,575.41</v>
       </c>
       <c r="E23" t="str">
-        <v>CORBL/9666/2,422.47</v>
+        <v>AHPC/59914/296.52</v>
       </c>
       <c r="F23" t="str">
-        <v>UNHPL/53220/398.10</v>
+        <v>SHIVM/23841/524.08</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="str">
-        <v>B29</v>
+        <v>B32</v>
       </c>
       <c r="B24" t="str">
-        <v>BPCL/108792/690.85</v>
+        <v>CHDC/30877/2,588.51</v>
       </c>
       <c r="C24" t="str">
-        <v>GRDBL/19732/1,267.53</v>
+        <v>CGH/53880/984.79</v>
       </c>
       <c r="D24" t="str">
-        <v>CHDC/7028/2,575.41</v>
+        <v>NRIC/41051/1,280.32</v>
       </c>
       <c r="E24" t="str">
-        <v>AHPC/59914/296.52</v>
+        <v>SHL/76769/579.60</v>
       </c>
       <c r="F24" t="str">
-        <v>SHIVM/23841/524.08</v>
+        <v>BARUN/81978/385.61</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="str">
-        <v>B32</v>
+        <v>B33</v>
       </c>
       <c r="B25" t="str">
-        <v>CHDC/30877/2,588.51</v>
+        <v>SBL/593960/297.39</v>
       </c>
       <c r="C25" t="str">
-        <v>CGH/53880/984.79</v>
+        <v>UPCL/185701/456.05</v>
       </c>
       <c r="D25" t="str">
-        <v>NRIC/41051/1,280.32</v>
+        <v>CHCL/130371/569.21</v>
       </c>
       <c r="E25" t="str">
-        <v>SHL/76769/579.60</v>
+        <v>EBL/94050/652.67</v>
       </c>
       <c r="F25" t="str">
-        <v>BARUN/81978/385.61</v>
+        <v>CBBL/40152/905.27</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="str">
-        <v>B33</v>
+        <v>B34</v>
       </c>
       <c r="B26" t="str">
-        <v>SBL/593960/297.39</v>
+        <v>SHPC/252687/616.01</v>
       </c>
       <c r="C26" t="str">
-        <v>UPCL/185701/456.05</v>
+        <v>RADHI/93130/798.51</v>
       </c>
       <c r="D26" t="str">
-        <v>CHCL/130371/569.21</v>
+        <v>HRL/71880/960.76</v>
       </c>
       <c r="E26" t="str">
-        <v>EBL/94050/652.67</v>
+        <v>SHIVM/87487/523.55</v>
       </c>
       <c r="F26" t="str">
-        <v>CBBL/40152/905.27</v>
+        <v>API/136033/301.74</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="str">
-        <v>B34</v>
+        <v>B35</v>
       </c>
       <c r="B27" t="str">
-        <v>SHPC/252687/616.01</v>
+        <v>GBIME/271020/240.05</v>
       </c>
       <c r="C27" t="str">
-        <v>RADHI/93130/798.51</v>
+        <v>UPCL/144728/446.06</v>
       </c>
       <c r="D27" t="str">
-        <v>HRL/71880/960.76</v>
+        <v>SBL/108577/299.05</v>
       </c>
       <c r="E27" t="str">
-        <v>SHIVM/87487/523.55</v>
+        <v>HURJA/102602/263.20</v>
       </c>
       <c r="F27" t="str">
-        <v>API/136033/301.74</v>
+        <v>CGH/29350/921.57</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="str">
-        <v>B35</v>
+        <v>B36</v>
       </c>
       <c r="B28" t="str">
-        <v>GBIME/271020/240.05</v>
+        <v>SBI/169393/411.44</v>
       </c>
       <c r="C28" t="str">
-        <v>UPCL/144728/446.06</v>
+        <v>SPDL/61525/417.69</v>
       </c>
       <c r="D28" t="str">
-        <v>SBL/108577/299.05</v>
+        <v>SHPC/34106/618.45</v>
       </c>
       <c r="E28" t="str">
-        <v>HURJA/102602/263.20</v>
+        <v>BARUN/35215/395.25</v>
       </c>
       <c r="F28" t="str">
-        <v>CGH/29350/921.57</v>
+        <v>KBL/57854/214.35</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="str">
-        <v>B36</v>
+        <v>B37</v>
       </c>
       <c r="B29" t="str">
-        <v>SBI/169393/411.44</v>
+        <v>MEN/9844/596.47</v>
       </c>
       <c r="C29" t="str">
-        <v>SPDL/61525/417.69</v>
+        <v>NRN/2150/2,068.32</v>
       </c>
       <c r="D29" t="str">
-        <v>SHPC/34106/618.45</v>
+        <v>BHPL/3885/951.93</v>
       </c>
       <c r="E29" t="str">
-        <v>BARUN/35215/395.25</v>
+        <v>MNBBL/8654/364.87</v>
       </c>
       <c r="F29" t="str">
-        <v>KBL/57854/214.35</v>
+        <v>MBJC/10060/310.87</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="str">
-        <v>B37</v>
+        <v>B38</v>
       </c>
       <c r="B30" t="str">
-        <v>MEN/9844/596.47</v>
+        <v>BPCL/252160/621.21</v>
       </c>
       <c r="C30" t="str">
-        <v>NRN/2150/2,068.32</v>
+        <v>SHIVM/82572/523.21</v>
       </c>
       <c r="D30" t="str">
-        <v>BHPL/3885/951.93</v>
+        <v>HPPL/69893/520.21</v>
       </c>
       <c r="E30" t="str">
-        <v>MNBBL/8654/364.87</v>
+        <v>SHL/48774/574.47</v>
       </c>
       <c r="F30" t="str">
-        <v>MBJC/10060/310.87</v>
+        <v>MBJC/80916/331.39</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="str">
-        <v>B38</v>
+        <v>B39</v>
       </c>
       <c r="B31" t="str">
-        <v>BPCL/252160/621.21</v>
+        <v>RADHI/275243/814.39</v>
       </c>
       <c r="C31" t="str">
-        <v>SHIVM/82572/523.21</v>
+        <v>NRN/33142/2,055.75</v>
       </c>
       <c r="D31" t="str">
-        <v>HPPL/69893/520.21</v>
+        <v>HPPL/100152/551.02</v>
       </c>
       <c r="E31" t="str">
-        <v>SHL/48774/574.47</v>
+        <v>UPCL/136084/439.98</v>
       </c>
       <c r="F31" t="str">
-        <v>MBJC/80916/331.39</v>
+        <v>AKPL/61901/278.91</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="str">
-        <v>B39</v>
+        <v>B40</v>
       </c>
       <c r="B32" t="str">
-        <v>RADHI/275243/814.39</v>
+        <v>BPCL/76358/622.40</v>
       </c>
       <c r="C32" t="str">
-        <v>NRN/33142/2,055.75</v>
+        <v>SANIMA/46798/318.19</v>
       </c>
       <c r="D32" t="str">
-        <v>HPPL/100152/551.02</v>
+        <v>EBL/20102/645.64</v>
       </c>
       <c r="E32" t="str">
-        <v>UPCL/136084/439.98</v>
+        <v>SHIVM/24218/522.24</v>
       </c>
       <c r="F32" t="str">
-        <v>AKPL/61901/278.91</v>
+        <v>RURU/11077/699.54</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="str">
-        <v>B40</v>
+        <v>B41</v>
       </c>
       <c r="B33" t="str">
-        <v>BPCL/76358/622.40</v>
+        <v>SAPDBL/140605/1,031.77</v>
       </c>
       <c r="C33" t="str">
-        <v>SANIMA/46798/318.19</v>
+        <v>RADHI/62622/807.75</v>
       </c>
       <c r="D33" t="str">
-        <v>EBL/20102/645.64</v>
+        <v>NMIC/18357/1,861.05</v>
       </c>
       <c r="E33" t="str">
-        <v>SHIVM/24218/522.24</v>
+        <v>SHIVM/45328/523.04</v>
       </c>
       <c r="F33" t="str">
-        <v>RURU/11077/699.54</v>
+        <v>BARUN/34740/387.37</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="str">
-        <v>B41</v>
+        <v>B42</v>
       </c>
       <c r="B34" t="str">
-        <v>SAPDBL/140605/1,031.77</v>
+        <v>GBIME/1038391/240.31</v>
       </c>
       <c r="C34" t="str">
-        <v>RADHI/62622/807.75</v>
+        <v>NRN/40244/2,022.50</v>
       </c>
       <c r="D34" t="str">
-        <v>NMIC/18357/1,861.05</v>
+        <v>MERO/94300/745.37</v>
       </c>
       <c r="E34" t="str">
-        <v>SHIVM/45328/523.04</v>
+        <v>SHIVM/116733/522.20</v>
       </c>
       <c r="F34" t="str">
-        <v>BARUN/34740/387.37</v>
+        <v>BARUN/107680/390.87</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="str">
-        <v>B42</v>
+        <v>B43</v>
       </c>
       <c r="B35" t="str">
-        <v>GBIME/1038391/240.31</v>
+        <v>SPDL/79440/424.46</v>
       </c>
       <c r="C35" t="str">
-        <v>NRN/40244/2,022.50</v>
+        <v>SPIL/24618/825.28</v>
       </c>
       <c r="D35" t="str">
-        <v>MERO/94300/745.37</v>
+        <v>USLB/8389/1,979.59</v>
       </c>
       <c r="E35" t="str">
-        <v>SHIVM/116733/522.20</v>
+        <v>MEN/24467/603.51</v>
       </c>
       <c r="F35" t="str">
-        <v>BARUN/107680/390.87</v>
+        <v>SHL/22773/571.84</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="str">
-        <v>B43</v>
+        <v>B44</v>
       </c>
       <c r="B36" t="str">
-        <v>SPDL/79440/424.46</v>
+        <v>CHCL/198483/568.71</v>
       </c>
       <c r="C36" t="str">
-        <v>SPIL/24618/825.28</v>
+        <v>NIFRA/238477/284.68</v>
       </c>
       <c r="D36" t="str">
-        <v>USLB/8389/1,979.59</v>
+        <v>EBL/103389/652.08</v>
       </c>
       <c r="E36" t="str">
-        <v>MEN/24467/603.51</v>
+        <v>UPCL/110590/451.34</v>
       </c>
       <c r="F36" t="str">
-        <v>SHL/22773/571.84</v>
+        <v>SANIMA/128386/320.98</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="str">
-        <v>B44</v>
+        <v>B45</v>
       </c>
       <c r="B37" t="str">
-        <v>CHCL/198483/568.71</v>
+        <v>MEN/171507/601.16</v>
       </c>
       <c r="C37" t="str">
-        <v>NIFRA/238477/284.68</v>
+        <v>GBIME/255156/226.30</v>
       </c>
       <c r="D37" t="str">
-        <v>EBL/103389/652.08</v>
+        <v>SHL/88816/572.71</v>
       </c>
       <c r="E37" t="str">
-        <v>UPCL/110590/451.34</v>
+        <v>CZBIL/192061/216.11</v>
       </c>
       <c r="F37" t="str">
-        <v>SANIMA/128386/320.98</v>
+        <v>SHPC/83154/601.97</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="str">
-        <v>B45</v>
+        <v>B46</v>
       </c>
       <c r="B38" t="str">
-        <v>MEN/171507/601.16</v>
+        <v>HRL/19693/939.21</v>
       </c>
       <c r="C38" t="str">
-        <v>GBIME/255156/226.30</v>
+        <v>SHPC/24665/615.06</v>
       </c>
       <c r="D38" t="str">
-        <v>SHL/88816/572.71</v>
+        <v>AHPC/38298/303.78</v>
       </c>
       <c r="E38" t="str">
-        <v>CZBIL/192061/216.11</v>
+        <v>SARBTM/13612/840.42</v>
       </c>
       <c r="F38" t="str">
-        <v>SHPC/83154/601.97</v>
+        <v>CREST/4676/1,775.23</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="str">
-        <v>B46</v>
+        <v>B47</v>
       </c>
       <c r="B39" t="str">
-        <v>HRL/19693/939.21</v>
+        <v>AKPL/150608/274.91</v>
       </c>
       <c r="C39" t="str">
-        <v>SHPC/24665/615.06</v>
+        <v>NGPL/90592/397.60</v>
       </c>
       <c r="D39" t="str">
-        <v>AHPC/38298/303.78</v>
+        <v>NRN/6825/2,037.60</v>
       </c>
       <c r="E39" t="str">
-        <v>SARBTM/13612/840.42</v>
+        <v>CREST/7901/1,728.25</v>
       </c>
       <c r="F39" t="str">
-        <v>CREST/4676/1,775.23</v>
+        <v>CHDC/4491/2,631.51</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="str">
-        <v>B47</v>
+        <v>B48</v>
       </c>
       <c r="B40" t="str">
-        <v>AKPL/150608/274.91</v>
+        <v>GHL/370313/264.13</v>
       </c>
       <c r="C40" t="str">
-        <v>NGPL/90592/397.60</v>
+        <v>SHIVM/88010/522.74</v>
       </c>
       <c r="D40" t="str">
-        <v>NRN/6825/2,037.60</v>
+        <v>MEN/70258/626.26</v>
       </c>
       <c r="E40" t="str">
-        <v>CREST/7901/1,728.25</v>
+        <v>HPPL/67387/559.44</v>
       </c>
       <c r="F40" t="str">
-        <v>CHDC/4491/2,631.51</v>
+        <v>NGPL/101956/392.88</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="str">
-        <v>B48</v>
+        <v>B49</v>
       </c>
       <c r="B41" t="str">
-        <v>GHL/370313/264.13</v>
+        <v>SHEL/191907/283.85</v>
       </c>
       <c r="C41" t="str">
-        <v>SHIVM/88010/522.74</v>
+        <v>RADHI/42924/792.39</v>
       </c>
       <c r="D41" t="str">
-        <v>MEN/70258/626.26</v>
+        <v>NGPL/81132/395.18</v>
       </c>
       <c r="E41" t="str">
-        <v>HPPL/67387/559.44</v>
+        <v>SHIVM/62955/523.38</v>
       </c>
       <c r="F41" t="str">
-        <v>NGPL/101956/392.88</v>
+        <v>API/106144/301.56</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="str">
-        <v>B49</v>
+        <v>B50</v>
       </c>
       <c r="B42" t="str">
-        <v>SHEL/191907/283.85</v>
+        <v>RADHI/436410/795.52</v>
       </c>
       <c r="C42" t="str">
-        <v>RADHI/42924/792.39</v>
+        <v>SHEL/124861/293.46</v>
       </c>
       <c r="D42" t="str">
-        <v>NGPL/81132/395.18</v>
+        <v>NGPL/104877/388.24</v>
       </c>
       <c r="E42" t="str">
-        <v>SHIVM/62955/523.38</v>
+        <v>SHL/49129/577.39</v>
       </c>
       <c r="F42" t="str">
-        <v>API/106144/301.56</v>
+        <v>AHPC/63297/297.72</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="str">
-        <v>B50</v>
+        <v>B51</v>
       </c>
       <c r="B43" t="str">
-        <v>RADHI/436410/795.52</v>
+        <v>CHDC/8571/2,608.31</v>
       </c>
       <c r="C43" t="str">
-        <v>SHEL/124861/293.46</v>
+        <v>AHPC/61953/299.33</v>
       </c>
       <c r="D43" t="str">
-        <v>NGPL/104877/388.24</v>
+        <v>BARUN/45823/391.67</v>
       </c>
       <c r="E43" t="str">
-        <v>SHL/49129/577.39</v>
+        <v>RADHI/21693/799.03</v>
       </c>
       <c r="F43" t="str">
-        <v>AHPC/63297/297.72</v>
+        <v>AKPL/47813/265.43</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="str">
-        <v>B51</v>
+        <v>B52</v>
       </c>
       <c r="B44" t="str">
-        <v>CHDC/8571/2,608.31</v>
+        <v>HIDCLP/127549/215.96</v>
       </c>
       <c r="C44" t="str">
-        <v>AHPC/61953/299.33</v>
+        <v>CHDC/8488/2,602.53</v>
       </c>
       <c r="D44" t="str">
-        <v>BARUN/45823/391.67</v>
+        <v>SHPC/32022/606.18</v>
       </c>
       <c r="E44" t="str">
-        <v>RADHI/21693/799.03</v>
+        <v>SHIVM/24974/522.06</v>
       </c>
       <c r="F44" t="str">
-        <v>AKPL/47813/265.43</v>
+        <v>NRN/6392/2,028.22</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="str">
-        <v>B52</v>
+        <v>B53</v>
       </c>
       <c r="B45" t="str">
-        <v>HIDCLP/127549/215.96</v>
+        <v>SHEL/34395/283.75</v>
       </c>
       <c r="C45" t="str">
-        <v>CHDC/8488/2,602.53</v>
+        <v>MLBL/24882/393.53</v>
       </c>
       <c r="D45" t="str">
-        <v>SHPC/32022/606.18</v>
+        <v>ULBSL/2548/3,346.70</v>
       </c>
       <c r="E45" t="str">
-        <v>SHIVM/24974/522.06</v>
+        <v>HURJA/30837/262.63</v>
       </c>
       <c r="F45" t="str">
-        <v>NRN/6392/2,028.22</v>
+        <v>MEN/13009/611.40</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="str">
-        <v>B53</v>
+        <v>B54</v>
       </c>
       <c r="B46" t="str">
-        <v>SHEL/34395/283.75</v>
+        <v>UPCL/205562/466.34</v>
       </c>
       <c r="C46" t="str">
-        <v>MLBL/24882/393.53</v>
+        <v>STC/14321/5,002.89</v>
       </c>
       <c r="D46" t="str">
-        <v>ULBSL/2548/3,346.70</v>
+        <v>CHCL/38572/562.68</v>
       </c>
       <c r="E46" t="str">
-        <v>HURJA/30837/262.63</v>
+        <v>CYCL/7011/1,669.84</v>
       </c>
       <c r="F46" t="str">
-        <v>MEN/13009/611.40</v>
+        <v>SADBL/24191/425.13</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="str">
-        <v>B54</v>
+        <v>B55</v>
       </c>
       <c r="B47" t="str">
-        <v>UPCL/205562/466.34</v>
+        <v>GMLI/139921/2,574.55</v>
       </c>
       <c r="C47" t="str">
-        <v>STC/14321/5,002.89</v>
+        <v>NRIC/261858/1,295.52</v>
       </c>
       <c r="D47" t="str">
-        <v>CHCL/38572/562.68</v>
+        <v>NMIC/95107/1,826.45</v>
       </c>
       <c r="E47" t="str">
-        <v>CYCL/7011/1,669.84</v>
+        <v>NLG/116518/828.81</v>
       </c>
       <c r="F47" t="str">
-        <v>SADBL/24191/425.13</v>
+        <v>HRL/34217/947.28</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="str">
-        <v>B55</v>
+        <v>B56</v>
       </c>
       <c r="B48" t="str">
-        <v>GMLI/139921/2,574.55</v>
+        <v>NGPL/210587/401.75</v>
       </c>
       <c r="C48" t="str">
-        <v>NRIC/261858/1,295.52</v>
+        <v>BPCL/108758/699.37</v>
       </c>
       <c r="D48" t="str">
-        <v>NMIC/95107/1,826.45</v>
+        <v>UPCL/153976/458.52</v>
       </c>
       <c r="E48" t="str">
-        <v>NLG/116518/828.81</v>
+        <v>HIDCLP/166359/218.89</v>
       </c>
       <c r="F48" t="str">
-        <v>HRL/34217/947.28</v>
+        <v>SMHL/36815/1,000.35</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="str">
-        <v>B56</v>
+        <v>B57</v>
       </c>
       <c r="B49" t="str">
-        <v>NGPL/210587/401.75</v>
+        <v>CHCL/74172/565.34</v>
       </c>
       <c r="C49" t="str">
-        <v>BPCL/108758/699.37</v>
+        <v>MEN/53613/606.78</v>
       </c>
       <c r="D49" t="str">
-        <v>UPCL/153976/458.52</v>
+        <v>UPCL/61470/452.15</v>
       </c>
       <c r="E49" t="str">
-        <v>HIDCLP/166359/218.89</v>
+        <v>NTC/28725/854.27</v>
       </c>
       <c r="F49" t="str">
-        <v>SMHL/36815/1,000.35</v>
+        <v>AHPC/78290/297.79</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="str">
-        <v>B57</v>
+        <v>B58</v>
       </c>
       <c r="B50" t="str">
-        <v>CHCL/74172/565.34</v>
+        <v>KBL/1211097/214.18</v>
       </c>
       <c r="C50" t="str">
-        <v>MEN/53613/606.78</v>
+        <v>NRN/93316/2,032.23</v>
       </c>
       <c r="D50" t="str">
-        <v>UPCL/61470/452.15</v>
+        <v>HPPL/309614/535.25</v>
       </c>
       <c r="E50" t="str">
-        <v>NTC/28725/854.27</v>
+        <v>HIDCLP/752979/218.77</v>
       </c>
       <c r="F50" t="str">
-        <v>AHPC/78290/297.79</v>
+        <v>LSL/461366/220.53</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="str">
-        <v>B58</v>
+        <v>B59</v>
       </c>
       <c r="B51" t="str">
-        <v>KBL/1211097/214.18</v>
+        <v>API/169244/302.19</v>
       </c>
       <c r="C51" t="str">
-        <v>NRN/93316/2,032.23</v>
+        <v>SHIVM/48234/522.99</v>
       </c>
       <c r="D51" t="str">
-        <v>HPPL/309614/535.25</v>
+        <v>AHPC/57092/301.40</v>
       </c>
       <c r="E51" t="str">
-        <v>HIDCLP/752979/218.77</v>
+        <v>ALICL/23360/681.11</v>
       </c>
       <c r="F51" t="str">
-        <v>LSL/461366/220.53</v>
+        <v>HIDCLP/65146/213.78</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="str">
-        <v>B59</v>
+        <v>B60</v>
       </c>
       <c r="B52" t="str">
-        <v>API/169244/302.19</v>
+        <v>RADHI/126847/802.14</v>
       </c>
       <c r="C52" t="str">
-        <v>SHIVM/48234/522.99</v>
+        <v>SHPC/123701/629.38</v>
       </c>
       <c r="D52" t="str">
-        <v>AHPC/57092/301.40</v>
+        <v>SHL/105682/577.34</v>
       </c>
       <c r="E52" t="str">
-        <v>ALICL/23360/681.11</v>
+        <v>HPPL/85782/528.62</v>
       </c>
       <c r="F52" t="str">
-        <v>HIDCLP/65146/213.78</v>
+        <v>BPCL/48140/687.40</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="str">
-        <v>B60</v>
+        <v>B61</v>
       </c>
       <c r="B53" t="str">
-        <v>RADHI/126847/802.14</v>
+        <v>RADHI/49172/814.95</v>
       </c>
       <c r="C53" t="str">
-        <v>SHPC/123701/629.38</v>
+        <v>NGPL/58310/400.53</v>
       </c>
       <c r="D53" t="str">
-        <v>SHL/105682/577.34</v>
+        <v>CHDC/8109/2,617.28</v>
       </c>
       <c r="E53" t="str">
-        <v>HPPL/85782/528.62</v>
+        <v>HIDCL/54149/308.72</v>
       </c>
       <c r="F53" t="str">
-        <v>BPCL/48140/687.40</v>
+        <v>HIDCLP/51753/218.27</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="str">
-        <v>B61</v>
+        <v>B62</v>
       </c>
       <c r="B54" t="str">
-        <v>RADHI/49172/814.95</v>
+        <v>UMHL/278829/515.17</v>
       </c>
       <c r="C54" t="str">
-        <v>NGPL/58310/400.53</v>
+        <v>UNHPL/259192/383.17</v>
       </c>
       <c r="D54" t="str">
-        <v>CHDC/8109/2,617.28</v>
+        <v>RADHI/68541/799.30</v>
       </c>
       <c r="E54" t="str">
-        <v>HIDCL/54149/308.72</v>
+        <v>SPDL/100762/417.88</v>
       </c>
       <c r="F54" t="str">
-        <v>HIDCLP/51753/218.27</v>
+        <v>ANLB/4513/5,394.85</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="str">
-        <v>B62</v>
+        <v>B63</v>
       </c>
       <c r="B55" t="str">
-        <v>UMHL/278829/515.17</v>
+        <v>RADHI/48086/798.33</v>
       </c>
       <c r="C55" t="str">
-        <v>UNHPL/259192/383.17</v>
+        <v>OMPL/11938/1,718.00</v>
       </c>
       <c r="D55" t="str">
-        <v>RADHI/68541/799.30</v>
+        <v>PPCL/40957/335.26</v>
       </c>
       <c r="E55" t="str">
-        <v>SPDL/100762/417.88</v>
+        <v>CHCL/20597/554.06</v>
       </c>
       <c r="F55" t="str">
-        <v>ANLB/4513/5,394.85</v>
+        <v>KBL/42191/212.13</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="str">
-        <v>B63</v>
+        <v>B64</v>
       </c>
       <c r="B56" t="str">
-        <v>RADHI/48086/798.33</v>
+        <v>BPCL/394960/641.39</v>
       </c>
       <c r="C56" t="str">
-        <v>OMPL/11938/1,718.00</v>
+        <v>NRN/19401/2,063.92</v>
       </c>
       <c r="D56" t="str">
-        <v>PPCL/40957/335.26</v>
+        <v>SHL/53841/581.25</v>
       </c>
       <c r="E56" t="str">
-        <v>CHCL/20597/554.06</v>
+        <v>UNHPL/77062/399.14</v>
       </c>
       <c r="F56" t="str">
-        <v>KBL/42191/212.13</v>
+        <v>CHDC/8801/2,564.03</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="str">
-        <v>B64</v>
+        <v>B65</v>
       </c>
       <c r="B57" t="str">
-        <v>BPCL/394960/641.39</v>
+        <v>SARBTM/54580/841.33</v>
       </c>
       <c r="C57" t="str">
-        <v>NRN/19401/2,063.92</v>
+        <v>RFPL/72961/623.28</v>
       </c>
       <c r="D57" t="str">
-        <v>SHL/53841/581.25</v>
+        <v>NIFRA/125622/282.74</v>
       </c>
       <c r="E57" t="str">
-        <v>UNHPL/77062/399.14</v>
+        <v>SANIMA/106987/318.67</v>
       </c>
       <c r="F57" t="str">
-        <v>CHDC/8801/2,564.03</v>
+        <v>SHPC/54334/607.97</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="str">
-        <v>B65</v>
+        <v>B66</v>
       </c>
       <c r="B58" t="str">
-        <v>SARBTM/54580/841.33</v>
+        <v>HIDCL/96377/304.77</v>
       </c>
       <c r="C58" t="str">
-        <v>RFPL/72961/623.28</v>
+        <v>CHDC/7582/2,589.41</v>
       </c>
       <c r="D58" t="str">
-        <v>NIFRA/125622/282.74</v>
+        <v>BPCL/29594/650.73</v>
       </c>
       <c r="E58" t="str">
-        <v>SANIMA/106987/318.67</v>
+        <v>NRN/7032/2,026.69</v>
       </c>
       <c r="F58" t="str">
-        <v>SHPC/54334/607.97</v>
+        <v>NGPL/34911/383.38</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="str">
-        <v>B66</v>
+        <v>B67</v>
       </c>
       <c r="B59" t="str">
-        <v>HIDCL/96377/304.77</v>
+        <v>RADHI/152046/785.65</v>
       </c>
       <c r="C59" t="str">
-        <v>CHDC/7582/2,589.41</v>
+        <v>HIDCL/168201/303.93</v>
       </c>
       <c r="D59" t="str">
-        <v>BPCL/29594/650.73</v>
+        <v>MEN/45354/621.45</v>
       </c>
       <c r="E59" t="str">
-        <v>NRN/7032/2,026.69</v>
+        <v>UMHL/49617/511.37</v>
       </c>
       <c r="F59" t="str">
-        <v>NGPL/34911/383.38</v>
+        <v>NGPL/48829/395.75</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="str">
-        <v>B67</v>
+        <v>B68</v>
       </c>
       <c r="B60" t="str">
-        <v>RADHI/152046/785.65</v>
+        <v>HIDCLP/216641/211.44</v>
       </c>
       <c r="C60" t="str">
-        <v>HIDCL/168201/303.93</v>
+        <v>NGPL/80704/386.86</v>
       </c>
       <c r="D60" t="str">
-        <v>MEN/45354/621.45</v>
+        <v>BPCL/28930/596.19</v>
       </c>
       <c r="E60" t="str">
-        <v>UMHL/49617/511.37</v>
+        <v>AHPC/53523/299.27</v>
       </c>
       <c r="F60" t="str">
-        <v>NGPL/48829/395.75</v>
+        <v>RIDI/58755/263.48</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="str">
-        <v>B68</v>
+        <v>B69</v>
       </c>
       <c r="B61" t="str">
-        <v>HIDCLP/216641/211.44</v>
+        <v>BPCL/92814/700.05</v>
       </c>
       <c r="C61" t="str">
-        <v>NGPL/80704/386.86</v>
+        <v>SHL/87203/576.55</v>
       </c>
       <c r="D61" t="str">
-        <v>BPCL/28930/596.19</v>
+        <v>SPDL/53053/427.77</v>
       </c>
       <c r="E61" t="str">
-        <v>AHPC/53523/299.27</v>
+        <v>SHEL/47740/288.79</v>
       </c>
       <c r="F61" t="str">
-        <v>RIDI/58755/263.48</v>
+        <v>NRN/5772/2,029.68</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="str">
-        <v>B69</v>
+        <v>B70</v>
       </c>
       <c r="B62" t="str">
-        <v>BPCL/92814/700.05</v>
+        <v>UNHPL/76391/390.07</v>
       </c>
       <c r="C62" t="str">
-        <v>SHL/87203/576.55</v>
+        <v>BPCL/55265/624.21</v>
       </c>
       <c r="D62" t="str">
-        <v>SPDL/53053/427.77</v>
+        <v>PRVU/79090/217.43</v>
       </c>
       <c r="E62" t="str">
-        <v>SHEL/47740/288.79</v>
+        <v>RADHI/19828/793.67</v>
       </c>
       <c r="F62" t="str">
-        <v>NRN/5772/2,029.68</v>
+        <v>UPCL/29417/451.12</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="str">
-        <v>B70</v>
+        <v>B71</v>
       </c>
       <c r="B63" t="str">
-        <v>UNHPL/76391/390.07</v>
+        <v>CHDC/8791/2,603.94</v>
       </c>
       <c r="C63" t="str">
-        <v>BPCL/55265/624.21</v>
+        <v>HIDCL/64871/311.05</v>
       </c>
       <c r="D63" t="str">
-        <v>PRVU/79090/217.43</v>
+        <v>SHPC/22754/642.47</v>
       </c>
       <c r="E63" t="str">
-        <v>RADHI/19828/793.67</v>
+        <v>UPCL/34881/446.62</v>
       </c>
       <c r="F63" t="str">
-        <v>UPCL/29417/451.12</v>
+        <v>CORBL/4656/2,343.91</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="str">
-        <v>B71</v>
+        <v>B72</v>
       </c>
       <c r="B64" t="str">
-        <v>CHDC/8791/2,603.94</v>
+        <v>CORBL/38542/2,378.38</v>
       </c>
       <c r="C64" t="str">
-        <v>HIDCL/64871/311.05</v>
+        <v>SAPDBL/32219/992.64</v>
       </c>
       <c r="D64" t="str">
-        <v>SHPC/22754/642.47</v>
+        <v>NRN/7066/2,038.86</v>
       </c>
       <c r="E64" t="str">
-        <v>UPCL/34881/446.62</v>
+        <v>KBL/60299/208.32</v>
       </c>
       <c r="F64" t="str">
-        <v>CORBL/4656/2,343.91</v>
+        <v>LBBL/27251/447.53</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="str">
-        <v>B72</v>
+        <v>B73</v>
       </c>
       <c r="B65" t="str">
-        <v>CORBL/38542/2,378.38</v>
+        <v>TVCL/780/472.13</v>
       </c>
       <c r="C65" t="str">
-        <v>SAPDBL/32219/992.64</v>
+        <v>BHL/1400/211.96</v>
       </c>
       <c r="D65" t="str">
-        <v>NRN/7066/2,038.86</v>
+        <v>RHGCL/480/554.96</v>
       </c>
       <c r="E65" t="str">
-        <v>KBL/60299/208.32</v>
+        <v>CHDC/82/2,712.71</v>
       </c>
       <c r="F65" t="str">
-        <v>LBBL/27251/447.53</v>
+        <v>SONA/300/453.00</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="str">
-        <v>B73</v>
+        <v>B74</v>
       </c>
       <c r="B66" t="str">
-        <v>TVCL/780/472.13</v>
+        <v>RADHI/77870/826.60</v>
       </c>
       <c r="C66" t="str">
-        <v>BHL/1400/211.96</v>
+        <v>SAPDBL/29337/1,036.06</v>
       </c>
       <c r="D66" t="str">
-        <v>RHGCL/480/554.96</v>
+        <v>SKBBL/17033/802.67</v>
       </c>
       <c r="E66" t="str">
-        <v>CHDC/82/2,712.71</v>
+        <v>NABIL/19968/493.76</v>
       </c>
       <c r="F66" t="str">
-        <v>SONA/300/453.00</v>
+        <v>SMHL/8722/1,009.86</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="str">
-        <v>B74</v>
+        <v>B75</v>
       </c>
       <c r="B67" t="str">
-        <v>RADHI/77870/826.60</v>
+        <v>CGH/32559/995.08</v>
       </c>
       <c r="C67" t="str">
-        <v>SAPDBL/29337/1,036.06</v>
+        <v>HIDCLP/122420/222.31</v>
       </c>
       <c r="D67" t="str">
-        <v>SKBBL/17033/802.67</v>
+        <v>BPCL/37613/675.24</v>
       </c>
       <c r="E67" t="str">
-        <v>NABIL/19968/493.76</v>
+        <v>SHPC/26842/632.16</v>
       </c>
       <c r="F67" t="str">
-        <v>SMHL/8722/1,009.86</v>
+        <v>GBIME/36153/234.56</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="str">
-        <v>B75</v>
+        <v>B76</v>
       </c>
       <c r="B68" t="str">
-        <v>CGH/32559/995.08</v>
+        <v>BPCL/81506/733.54</v>
       </c>
       <c r="C68" t="str">
-        <v>HIDCLP/122420/222.31</v>
+        <v>SHIVM/21722/519.98</v>
       </c>
       <c r="D68" t="str">
-        <v>BPCL/37613/675.24</v>
+        <v>UMRH/6524/623.95</v>
       </c>
       <c r="E68" t="str">
-        <v>SHPC/26842/632.16</v>
+        <v>HIDCL/9386/314.43</v>
       </c>
       <c r="F68" t="str">
-        <v>GBIME/36153/234.56</v>
+        <v>MEN/4684/581.67</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="str">
-        <v>B76</v>
+        <v>B77</v>
       </c>
       <c r="B69" t="str">
-        <v>BPCL/81506/733.54</v>
+        <v>BPCL/279333/614.23</v>
       </c>
       <c r="C69" t="str">
-        <v>SHIVM/21722/519.98</v>
+        <v>NGPL/145469/402.86</v>
       </c>
       <c r="D69" t="str">
-        <v>UMRH/6524/623.95</v>
+        <v>AHPC/118928/306.46</v>
       </c>
       <c r="E69" t="str">
-        <v>HIDCL/9386/314.43</v>
+        <v>MEN/38568/615.00</v>
       </c>
       <c r="F69" t="str">
-        <v>MEN/4684/581.67</v>
+        <v>LBBL/48172/469.45</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="str">
-        <v>B77</v>
+        <v>B78</v>
       </c>
       <c r="B70" t="str">
-        <v>BPCL/279333/614.23</v>
+        <v>CHDC/2956/2,643.70</v>
       </c>
       <c r="C70" t="str">
-        <v>NGPL/145469/402.86</v>
+        <v>ALICL/7268/690.33</v>
       </c>
       <c r="D70" t="str">
-        <v>AHPC/118928/306.46</v>
+        <v>HIDCLP/20213/219.38</v>
       </c>
       <c r="E70" t="str">
-        <v>MEN/38568/615.00</v>
+        <v>NGPL/9699/396.24</v>
       </c>
       <c r="F70" t="str">
-        <v>LBBL/48172/469.45</v>
+        <v>SINDU/3020/855.60</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="str">
-        <v>B78</v>
+        <v>B79</v>
       </c>
       <c r="B71" t="str">
-        <v>CHDC/2956/2,643.70</v>
+        <v>SMPDA/1414/927.99</v>
       </c>
       <c r="C71" t="str">
-        <v>ALICL/7268/690.33</v>
+        <v>TRH/1200/946.50</v>
       </c>
       <c r="D71" t="str">
-        <v>HIDCLP/20213/219.38</v>
+        <v>AKPL/3096/272.99</v>
       </c>
       <c r="E71" t="str">
-        <v>NGPL/9699/396.24</v>
+        <v>SHIVM/1600/520.50</v>
       </c>
       <c r="F71" t="str">
-        <v>SINDU/3020/855.60</v>
+        <v>NGPL/1770/398.96</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="str">
-        <v>B79</v>
+        <v>B80</v>
       </c>
       <c r="B72" t="str">
-        <v>SMPDA/1414/927.99</v>
+        <v>NIFRA/95287/287.08</v>
       </c>
       <c r="C72" t="str">
-        <v>TRH/1200/946.50</v>
+        <v>NMLBBL/39463/658.87</v>
       </c>
       <c r="D72" t="str">
-        <v>AKPL/3096/272.99</v>
+        <v>CHCL/26361/551.37</v>
       </c>
       <c r="E72" t="str">
-        <v>SHIVM/1600/520.50</v>
+        <v>USLB/6883/1,849.41</v>
       </c>
       <c r="F72" t="str">
-        <v>NGPL/1770/398.96</v>
+        <v>MEN/22305/590.68</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="str">
-        <v>B80</v>
+        <v>B81</v>
       </c>
       <c r="B73" t="str">
-        <v>NIFRA/95287/287.08</v>
+        <v>CHCL/126508/562.89</v>
       </c>
       <c r="C73" t="str">
-        <v>NMLBBL/39463/658.87</v>
+        <v>NGPL/151977/395.77</v>
       </c>
       <c r="D73" t="str">
-        <v>CHCL/26361/551.37</v>
+        <v>HRL/44228/966.10</v>
       </c>
       <c r="E73" t="str">
-        <v>USLB/6883/1,849.41</v>
+        <v>SHPC/60307/606.42</v>
       </c>
       <c r="F73" t="str">
-        <v>MEN/22305/590.68</v>
+        <v>CHDC/10296/2,614.60</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="str">
-        <v>B81</v>
+        <v>B82</v>
       </c>
       <c r="B74" t="str">
-        <v>CHCL/126508/562.89</v>
+        <v>SHPC/52883/601.62</v>
       </c>
       <c r="C74" t="str">
-        <v>NGPL/151977/395.77</v>
+        <v>NRN/13502/2,043.78</v>
       </c>
       <c r="D74" t="str">
-        <v>HRL/44228/966.10</v>
+        <v>NICA/25422/372.12</v>
       </c>
       <c r="E74" t="str">
-        <v>SHPC/60307/606.42</v>
+        <v>HRL/10698/951.94</v>
       </c>
       <c r="F74" t="str">
-        <v>CHDC/10296/2,614.60</v>
+        <v>NLIC/12878/755.85</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="str">
-        <v>B82</v>
+        <v>B83</v>
       </c>
       <c r="B75" t="str">
-        <v>SHPC/52883/601.62</v>
+        <v>HRL/28887/942.77</v>
       </c>
       <c r="C75" t="str">
-        <v>NRN/13502/2,043.78</v>
+        <v>NGPL/53985/401.22</v>
       </c>
       <c r="D75" t="str">
-        <v>NICA/25422/372.12</v>
+        <v>SHPC/30230/626.19</v>
       </c>
       <c r="E75" t="str">
-        <v>HRL/10698/951.94</v>
+        <v>KPCL/20408/520.95</v>
       </c>
       <c r="F75" t="str">
-        <v>NLIC/12878/755.85</v>
+        <v>AHL/14385/674.65</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="str">
-        <v>B83</v>
+        <v>B84</v>
       </c>
       <c r="B76" t="str">
-        <v>HRL/28887/942.77</v>
+        <v>HIDCL/97416/308.24</v>
       </c>
       <c r="C76" t="str">
-        <v>NGPL/53985/401.22</v>
+        <v>UPCL/60805/451.77</v>
       </c>
       <c r="D76" t="str">
-        <v>SHPC/30230/626.19</v>
+        <v>BPCL/36467/703.94</v>
       </c>
       <c r="E76" t="str">
-        <v>KPCL/20408/520.95</v>
+        <v>SADBL/67875/421.04</v>
       </c>
       <c r="F76" t="str">
-        <v>AHL/14385/674.65</v>
+        <v>NGPL/56710/400.50</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="str">
-        <v>B84</v>
+        <v>B85</v>
       </c>
       <c r="B77" t="str">
-        <v>HIDCL/97416/308.24</v>
+        <v>NGPL/234021/385.35</v>
       </c>
       <c r="C77" t="str">
-        <v>UPCL/60805/451.77</v>
+        <v>SHL/66561/583.61</v>
       </c>
       <c r="D77" t="str">
-        <v>BPCL/36467/703.94</v>
+        <v>AHPC/75054/298.31</v>
       </c>
       <c r="E77" t="str">
-        <v>SADBL/67875/421.04</v>
+        <v>API/68186/302.76</v>
       </c>
       <c r="F77" t="str">
-        <v>NGPL/56710/400.50</v>
+        <v>SPDL/27097/412.50</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="str">
-        <v>B85</v>
+        <v>B86</v>
       </c>
       <c r="B78" t="str">
-        <v>NGPL/234021/385.35</v>
+        <v>RADHI/30445/801.14</v>
       </c>
       <c r="C78" t="str">
-        <v>SHL/66561/583.61</v>
+        <v>SHPC/25971/618.94</v>
       </c>
       <c r="D78" t="str">
-        <v>AHPC/75054/298.31</v>
+        <v>AKPL/28465/272.85</v>
       </c>
       <c r="E78" t="str">
-        <v>API/68186/302.76</v>
+        <v>NRN/3764/2,023.67</v>
       </c>
       <c r="F78" t="str">
-        <v>SPDL/27097/412.50</v>
+        <v>API/24420/299.70</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="str">
-        <v>B86</v>
+        <v>B87</v>
       </c>
       <c r="B79" t="str">
-        <v>RADHI/30445/801.14</v>
+        <v>BPCL/48449/741.54</v>
       </c>
       <c r="C79" t="str">
-        <v>SHPC/25971/618.94</v>
+        <v>RADHI/47373/803.90</v>
       </c>
       <c r="D79" t="str">
-        <v>AKPL/28465/272.85</v>
+        <v>CGH/6405/968.10</v>
       </c>
       <c r="E79" t="str">
-        <v>NRN/3764/2,023.67</v>
+        <v>AKPL/19752/281.20</v>
       </c>
       <c r="F79" t="str">
-        <v>API/24420/299.70</v>
+        <v>NGPL/17061/389.01</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="str">
-        <v>B87</v>
+        <v>B88</v>
       </c>
       <c r="B80" t="str">
-        <v>BPCL/48449/741.54</v>
+        <v>SAPDBL/60246/1,049.78</v>
       </c>
       <c r="C80" t="str">
-        <v>RADHI/47373/803.90</v>
+        <v>CHCL/56976/568.74</v>
       </c>
       <c r="D80" t="str">
-        <v>CGH/6405/968.10</v>
+        <v>CHDC/6030/2,583.14</v>
       </c>
       <c r="E80" t="str">
-        <v>AKPL/19752/281.20</v>
+        <v>CORBL/4693/2,617.66</v>
       </c>
       <c r="F80" t="str">
-        <v>NGPL/17061/389.01</v>
+        <v>NHPC/48131/223.39</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="str">
-        <v>B88</v>
+        <v>B89</v>
       </c>
       <c r="B81" t="str">
-        <v>SAPDBL/60246/1,049.78</v>
+        <v>GBIME/111393/238.71</v>
       </c>
       <c r="C81" t="str">
-        <v>CHCL/56976/568.74</v>
+        <v>BPCL/15296/689.78</v>
       </c>
       <c r="D81" t="str">
-        <v>CHDC/6030/2,583.14</v>
+        <v>CGH/7956/965.88</v>
       </c>
       <c r="E81" t="str">
-        <v>CORBL/4693/2,617.66</v>
+        <v>UNHPL/13561/412.68</v>
       </c>
       <c r="F81" t="str">
-        <v>NHPC/48131/223.39</v>
+        <v>MEN/8613/616.04</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="str">
-        <v>B89</v>
+        <v>B90</v>
       </c>
       <c r="B82" t="str">
-        <v>GBIME/111393/238.71</v>
+        <v>HBL/113377/229.39</v>
       </c>
       <c r="C82" t="str">
-        <v>BPCL/15296/689.78</v>
+        <v>API/58129/311.32</v>
       </c>
       <c r="D82" t="str">
-        <v>CGH/7956/965.88</v>
+        <v>EBL/11126/631.20</v>
       </c>
       <c r="E82" t="str">
-        <v>UNHPL/13561/412.68</v>
+        <v>LEC/20741/224.25</v>
       </c>
       <c r="F82" t="str">
-        <v>MEN/8613/616.04</v>
+        <v>UPCL/6382/441.13</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="str">
-        <v>B90</v>
+        <v>B91</v>
       </c>
       <c r="B83" t="str">
-        <v>HBL/113377/229.39</v>
+        <v>NGPL/62977/393.14</v>
       </c>
       <c r="C83" t="str">
-        <v>API/58129/311.32</v>
+        <v>RADHI/28104/795.91</v>
       </c>
       <c r="D83" t="str">
-        <v>EBL/11126/631.20</v>
+        <v>BPCL/29965/656.03</v>
       </c>
       <c r="E83" t="str">
-        <v>LEC/20741/224.25</v>
+        <v>SARBTM/17294/842.98</v>
       </c>
       <c r="F83" t="str">
-        <v>UPCL/6382/441.13</v>
+        <v>CHDC/5241/2,614.09</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="str">
-        <v>B91</v>
+        <v>B92</v>
       </c>
       <c r="B84" t="str">
-        <v>NGPL/62977/393.14</v>
+        <v>HIDCL/103329/304.19</v>
       </c>
       <c r="C84" t="str">
-        <v>RADHI/28104/795.91</v>
+        <v>UPCL/35717/450.94</v>
       </c>
       <c r="D84" t="str">
-        <v>BPCL/29965/656.03</v>
+        <v>BPCL/12087/673.28</v>
       </c>
       <c r="E84" t="str">
-        <v>SARBTM/17294/842.98</v>
+        <v>NGPL/18738/391.19</v>
       </c>
       <c r="F84" t="str">
-        <v>CHDC/5241/2,614.09</v>
+        <v>HRL/7529/956.96</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="str">
-        <v>B92</v>
+        <v>B93</v>
       </c>
       <c r="B85" t="str">
-        <v>HIDCL/103329/304.19</v>
+        <v>MBJC/21250/335.67</v>
       </c>
       <c r="C85" t="str">
-        <v>UPCL/35717/450.94</v>
+        <v>AKPL/20900/289.70</v>
       </c>
       <c r="D85" t="str">
-        <v>BPCL/12087/673.28</v>
+        <v>ICFC/5020/622.19</v>
       </c>
       <c r="E85" t="str">
-        <v>NGPL/18738/391.19</v>
+        <v>MPFL/4420/614.53</v>
       </c>
       <c r="F85" t="str">
-        <v>HRL/7529/956.96</v>
+        <v>CHCL/3227/545.51</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="str">
-        <v>B93</v>
+        <v>B94</v>
       </c>
       <c r="B86" t="str">
-        <v>MBJC/21250/335.67</v>
+        <v>RADHI/128662/792.47</v>
       </c>
       <c r="C86" t="str">
-        <v>AKPL/20900/289.70</v>
+        <v>SHL/41223/570.38</v>
       </c>
       <c r="D86" t="str">
-        <v>ICFC/5020/622.19</v>
+        <v>MKHL/29191/745.23</v>
       </c>
       <c r="E86" t="str">
-        <v>MPFL/4420/614.53</v>
+        <v>PRIN/17725/844.95</v>
       </c>
       <c r="F86" t="str">
-        <v>CHCL/3227/545.51</v>
+        <v>SHIVM/19328/519.38</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="str">
-        <v>B94</v>
+        <v>B95</v>
       </c>
       <c r="B87" t="str">
-        <v>RADHI/128662/792.47</v>
+        <v>NGPL/67372/398.02</v>
       </c>
       <c r="C87" t="str">
-        <v>SHL/41223/570.38</v>
+        <v>UPCL/45075/454.84</v>
       </c>
       <c r="D87" t="str">
-        <v>MKHL/29191/745.23</v>
+        <v>RADHI/18844/819.35</v>
       </c>
       <c r="E87" t="str">
-        <v>PRIN/17725/844.95</v>
+        <v>SHPC/23719/597.44</v>
       </c>
       <c r="F87" t="str">
-        <v>SHIVM/19328/519.38</v>
+        <v>NRN/5063/2,058.99</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="str">
-        <v>B95</v>
+        <v>B96</v>
       </c>
       <c r="B88" t="str">
-        <v>NGPL/67372/398.02</v>
+        <v>NRN/35354/2,043.52</v>
       </c>
       <c r="C88" t="str">
-        <v>UPCL/45075/454.84</v>
+        <v>NICA/104431/365.65</v>
       </c>
       <c r="D88" t="str">
-        <v>RADHI/18844/819.35</v>
+        <v>BPCL/45007/684.97</v>
       </c>
       <c r="E88" t="str">
-        <v>SHPC/23719/597.44</v>
+        <v>SHPC/49061/619.47</v>
       </c>
       <c r="F88" t="str">
-        <v>NRN/5063/2,058.99</v>
+        <v>RADHI/35532/824.05</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="str">
-        <v>B96</v>
+        <v>B97</v>
       </c>
       <c r="B89" t="str">
-        <v>NRN/35354/2,043.52</v>
+        <v>SADBL/23762/418.13</v>
       </c>
       <c r="C89" t="str">
-        <v>NICA/104431/365.65</v>
+        <v>NRN/4551/2,028.54</v>
       </c>
       <c r="D89" t="str">
-        <v>BPCL/45007/684.97</v>
+        <v>MEN/11700/633.74</v>
       </c>
       <c r="E89" t="str">
-        <v>SHPC/49061/619.47</v>
+        <v>UPCL/16179/451.50</v>
       </c>
       <c r="F89" t="str">
-        <v>RADHI/35532/824.05</v>
+        <v>SPDL/14296/401.84</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="str">
-        <v>B97</v>
+        <v>B98</v>
       </c>
       <c r="B90" t="str">
-        <v>SADBL/23762/418.13</v>
+        <v>BPCL/64464/746.92</v>
       </c>
       <c r="C90" t="str">
-        <v>NRN/4551/2,028.54</v>
+        <v>OMPL/8870/1,823.74</v>
       </c>
       <c r="D90" t="str">
-        <v>MEN/11700/633.74</v>
+        <v>AKPL/52329/283.73</v>
       </c>
       <c r="E90" t="str">
-        <v>UPCL/16179/451.50</v>
+        <v>SHIVM/11710/524.31</v>
       </c>
       <c r="F90" t="str">
-        <v>SPDL/14296/401.84</v>
+        <v>RIDI/20290/288.71</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="str">
-        <v>B98</v>
+        <v>B99</v>
       </c>
       <c r="B91" t="str">
-        <v>BPCL/64464/746.92</v>
+        <v>SHEL/51665/296.52</v>
       </c>
       <c r="C91" t="str">
-        <v>OMPL/8870/1,823.74</v>
+        <v>BPCL/15186/652.43</v>
       </c>
       <c r="D91" t="str">
-        <v>AKPL/52329/283.73</v>
+        <v>CGH/7486/992.83</v>
       </c>
       <c r="E91" t="str">
-        <v>SHIVM/11710/524.31</v>
+        <v>HIDCLP/30115/210.30</v>
       </c>
       <c r="F91" t="str">
-        <v>RIDI/20290/288.71</v>
+        <v>CHDC/2090/2,619.22</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="str">
-        <v>B99</v>
+        <v>B100</v>
       </c>
       <c r="B92" t="str">
-        <v>SHEL/51665/296.52</v>
+        <v>MLBL/153277/389.17</v>
       </c>
       <c r="C92" t="str">
-        <v>BPCL/15186/652.43</v>
+        <v>PHCL/44005/581.11</v>
       </c>
       <c r="D92" t="str">
-        <v>CGH/7486/992.83</v>
+        <v>KSBBL/51027/449.82</v>
       </c>
       <c r="E92" t="str">
-        <v>HIDCLP/30115/210.30</v>
+        <v>BPCL/29353/737.25</v>
       </c>
       <c r="F92" t="str">
-        <v>CHDC/2090/2,619.22</v>
+        <v>LBBL/44169/448.48</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="str">
-        <v>B100</v>
+        <v>B101</v>
       </c>
       <c r="B93" t="str">
-        <v>MLBL/153277/389.17</v>
+        <v>HIDCLP/56750/217.48</v>
       </c>
       <c r="C93" t="str">
-        <v>PHCL/44005/581.11</v>
+        <v>CHDC/4087/2,645.00</v>
       </c>
       <c r="D93" t="str">
-        <v>KSBBL/51027/449.82</v>
+        <v>AKPL/36877/276.61</v>
       </c>
       <c r="E93" t="str">
-        <v>BPCL/29353/737.25</v>
+        <v>AHPC/27574/307.21</v>
       </c>
       <c r="F93" t="str">
-        <v>LBBL/44169/448.48</v>
-      </c>
-    </row>
-    <row r="94">
-      <c r="A94" t="str">
-        <v>B101</v>
-      </c>
-      <c r="B94" t="str">
-        <v>HIDCLP/56750/217.48</v>
-      </c>
-      <c r="C94" t="str">
-        <v>CHDC/4087/2,645.00</v>
-      </c>
-      <c r="D94" t="str">
-        <v>AKPL/36877/276.61</v>
-      </c>
-      <c r="E94" t="str">
-        <v>AHPC/27574/307.21</v>
-      </c>
-      <c r="F94" t="str">
         <v>RADHI/9917/817.89</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F94"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F93"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>